<commit_message>
chore: Completed histogram & quantiles tutorials
</commit_message>
<xml_diff>
--- a/1.3_Methods_of_Descriptive_Statistics/Creating_a_Histogram.xlsx
+++ b/1.3_Methods_of_Descriptive_Statistics/Creating_a_Histogram.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vreed\Desktop\Ryan\AIEngineer\WGU\MSDA\D205_Data_Acquisition\1.3_Methods_of_Descriptive_Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7689B60-CA1E-4083-9203-A695A25853FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E916E137-A244-46B3-B337-6CB07442948C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA218F0A-BC8A-4F6F-9259-03E408F4A599}"/>
   </bookViews>
   <sheets>
-    <sheet name="heights" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
+    <sheet name="heights" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">heights!$A$1:$A$10001</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">heights!$A$1:$A$10001</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,17 +47,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>height</t>
+  </si>
+  <si>
+    <t>Bin</t>
+  </si>
+  <si>
+    <t>More</t>
+  </si>
+  <si>
+    <t>Frequency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -72,7 +90,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -80,12 +98,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -101,6 +145,329 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Heights</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Frequency</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$2:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>More</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1143</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1917</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1817</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1325</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ECFE-47EA-B240-CEE2EB449309}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1250679696"/>
+        <c:axId val="1250681360"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1250679696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Bin</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1250681360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1250681360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1250679696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8E4DB7A-CBCD-4CC6-B5D4-16F240ACFEF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,10 +786,182 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACCCC12-C8DA-4A5D-96C7-66408F8360DE}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>140</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>145</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>150</v>
+      </c>
+      <c r="B4" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>155</v>
+      </c>
+      <c r="B5" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>160</v>
+      </c>
+      <c r="B6" s="2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>165</v>
+      </c>
+      <c r="B7" s="2">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>170</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>175</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>180</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>185</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>190</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>195</v>
+      </c>
+      <c r="B13" s="2">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>200</v>
+      </c>
+      <c r="B14" s="2">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>205</v>
+      </c>
+      <c r="B15" s="2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>210</v>
+      </c>
+      <c r="B16" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>215</v>
+      </c>
+      <c r="B17" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>220</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A18">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E764039F-91F1-4FDD-902E-B6DC9A6E628B}">
   <dimension ref="A1:C10001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -50495,7 +51034,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{592AF37B-388D-4DE9-B5E5-AA790B4CFCDD}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>